<commit_message>
Excel test description updated
</commit_message>
<xml_diff>
--- a/Automation_Saucedemo/DataFiles/InputData.xlsx
+++ b/Automation_Saucedemo/DataFiles/InputData.xlsx
@@ -52,7 +52,7 @@
     <t>TC_001</t>
   </si>
   <si>
-    <t>Login as staff</t>
+    <t>TC_001 Checkout - Sauce Labs Bike Light</t>
   </si>
   <si>
     <t>Yes</t>
@@ -489,7 +489,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="131" zoomScaleNormal="100">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>

</xml_diff>